<commit_message>
Add .gitignore, add a function that saves all the products with special offers to properly fomatted gsheets
</commit_message>
<xml_diff>
--- a/sheets/shoper_all_special_offers.xlsx
+++ b/sheets/shoper_all_special_offers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>promo_id</t>
+          <t>code</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>discount_type</t>
+          <t>product_id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>discount</t>
+          <t>product_name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>discount_wholesale</t>
+          <t>price</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>discount_special</t>
+          <t>promo_price</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -467,437 +467,302 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>date_to</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>condition_type</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>product_id</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>stocks</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>745883670185</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6080</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10.00</t>
+          <t>Uchwyt samochodowy Belkin Car Cup Mount (do 83mm), czarny</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>169.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>149.00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-09-28 17:28:14</t>
+          <t>25-05-2023</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2024-11-28 17:28:14</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>[54]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5901571174976</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>8272</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>40.00</t>
+          <t>Folia ochronna 3mk Arc Microsoft Band 2, 3 szt.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>29.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>11.60</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-10-26 17:28:14</t>
+          <t>10-04-2024</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2024-12-28 17:28:14</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>[148]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8809565309809</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9847</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>30.00</t>
+          <t>Etui wodoszczelne Spigen Velo A600 IPX8  do telefonu max 16,3 x 9cm, białe</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>69.00</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>41.40</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-10-26 17:28:14</t>
+          <t>10-04-2024</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2024-12-28 17:28:14</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>[57]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>745883734108</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9876</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>25.00</t>
+          <t>Adapter Belkin MFi 3.5mm Audio + Charge RockStar, białe</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>205.00</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>159.00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-10-26 17:28:14</t>
+          <t>25-05-2023</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2024-12-28 17:28:14</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>79</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>[146]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5904538092801</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10855</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>22.00</t>
+          <t>Szkło hartowane na aparat Mocolo TG+ iPhone Xs/X</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>19.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>15.20</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-10-26 17:28:14</t>
+          <t>12-02-2024</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2024-12-28 17:28:14</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>[141]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5904538092825</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10858</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>140.00</t>
+          <t>Szkło hartowane na aparat Mocolo TG+ iPhone Xs Max</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>19.00</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7.60</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-10-26 17:28:14</t>
+          <t>08-01-2024</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2024-12-28 17:28:14</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>[143]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6953156257344</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11566</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10.00</t>
+          <t>Uchwyt samochodowy na telefon Baseus Gravity Type SUYL-01, czarny</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>49.00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35.00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-11-24 00:00:00</t>
+          <t>26-01-2025</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2026-01-01 23:59:59</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>10745</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>[10833]</t>
+          <t>01-12-2027</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8809613769999</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11619</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>20.00</t>
+          <t>Etui Spigen Liquid Air Galaxy A9 2018, matowe czarne</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>49.00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1.99</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-01-30 00:00:00</t>
+          <t>24-10-2022</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-02-09 23:59:59</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>10744</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>[10832]</t>
+          <t>31-12-2027</t>
         </is>
       </c>
     </row>

</xml_diff>